<commit_message>
Auswertung in text file und excel sheet angepasst
</commit_message>
<xml_diff>
--- a/UE2/UE2.xlsx
+++ b/UE2/UE2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="111">
   <si>
     <t>tn[s] </t>
   </si>
@@ -66,6 +66,300 @@
   </si>
   <si>
     <t>Betragspektren:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Signalanfang </t>
+  </si>
+  <si>
+    <t>DFT-Spektren (komplexe Zahlen):</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>0,00000000000000i</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>1,38430799185348i</t>
+  </si>
+  <si>
+    <t>3,05358869243304i</t>
+  </si>
+  <si>
+    <t>5,60767243907572i</t>
+  </si>
+  <si>
+    <t>11,1011025141367i</t>
+  </si>
+  <si>
+    <t>39,4156129226817i</t>
+  </si>
+  <si>
+    <t>36,3829111169553i</t>
+  </si>
+  <si>
+    <t>13,6892123541936i</t>
+  </si>
+  <si>
+    <t>8,64740157752124i</t>
+  </si>
+  <si>
+    <t>6,42408849652177i</t>
+  </si>
+  <si>
+    <t>5,09889515326748i</t>
+  </si>
+  <si>
+    <t>4,24987966138358i</t>
+  </si>
+  <si>
+    <t>3,59280408147751i</t>
+  </si>
+  <si>
+    <t>3,13074923418218i</t>
+  </si>
+  <si>
+    <t>2,72503904948595i</t>
+  </si>
+  <si>
+    <t>2,49108927812500i</t>
+  </si>
+  <si>
+    <t>2,07750000000000i</t>
+  </si>
+  <si>
+    <t>2,01329603731415i</t>
+  </si>
+  <si>
+    <t>1,77718836657622i</t>
+  </si>
+  <si>
+    <t>1,53320456218144i</t>
+  </si>
+  <si>
+    <t>1,39373827456025i</t>
+  </si>
+  <si>
+    <t>1,25724818796585i</t>
+  </si>
+  <si>
+    <t>1,11536282055434i</t>
+  </si>
+  <si>
+    <t>0,959428514837794i</t>
+  </si>
+  <si>
+    <t>0,839001577521241i</t>
+  </si>
+  <si>
+    <t>0,745162531065811i</t>
+  </si>
+  <si>
+    <t>0,611822539567488i</t>
+  </si>
+  <si>
+    <t>0,518871249237311i</t>
+  </si>
+  <si>
+    <t>0,397831678946076i</t>
+  </si>
+  <si>
+    <t>0,294310210626607i</t>
+  </si>
+  <si>
+    <t>0,198204379982533i</t>
+  </si>
+  <si>
+    <t>0,0917206022581392i</t>
+  </si>
+  <si>
+    <t>3,45202257613892i</t>
+  </si>
+  <si>
+    <t>3,72612191008443i</t>
+  </si>
+  <si>
+    <t>0,871013272112138i</t>
+  </si>
+  <si>
+    <t>3,76502449062203i</t>
+  </si>
+  <si>
+    <t>1,31743420649628i</t>
+  </si>
+  <si>
+    <t>8,19209727509782i</t>
+  </si>
+  <si>
+    <t>17,6525634269171i</t>
+  </si>
+  <si>
+    <t>16,3991807973877i</t>
+  </si>
+  <si>
+    <t>4,29869568411853i</t>
+  </si>
+  <si>
+    <t>3,25983670209807i</t>
+  </si>
+  <si>
+    <t>1,29797616887436i</t>
+  </si>
+  <si>
+    <t>1,01918715737308i</t>
+  </si>
+  <si>
+    <t>0,224952290177872i</t>
+  </si>
+  <si>
+    <t>0,194497133602410i</t>
+  </si>
+  <si>
+    <t>0,323092991140006i</t>
+  </si>
+  <si>
+    <t>0,123200000000000i</t>
+  </si>
+  <si>
+    <t>0,591607420598895i</t>
+  </si>
+  <si>
+    <t>0,574076669091726i</t>
+  </si>
+  <si>
+    <t>0,488117933817087i</t>
+  </si>
+  <si>
+    <t>0,419871603290322i</t>
+  </si>
+  <si>
+    <t>0,316434874613516i</t>
+  </si>
+  <si>
+    <t>0,249020982259202i</t>
+  </si>
+  <si>
+    <t>0,0473209959648107i</t>
+  </si>
+  <si>
+    <t>0,0339807973876809i</t>
+  </si>
+  <si>
+    <t>0,131214189345966i</t>
+  </si>
+  <si>
+    <t>0,137836602706433i</t>
+  </si>
+  <si>
+    <t>0,207926652858794i</t>
+  </si>
+  <si>
+    <t>0,201516748714564i</t>
+  </si>
+  <si>
+    <t>0,186923483106459i</t>
+  </si>
+  <si>
+    <t>0,125695849382948i</t>
+  </si>
+  <si>
+    <t>0,0889109751727459i</t>
+  </si>
+  <si>
+    <t>1,22335758912438i</t>
+  </si>
+  <si>
+    <t>58,1466262471765i</t>
+  </si>
+  <si>
+    <t>1,09060314234862i</t>
+  </si>
+  <si>
+    <t>0,300604841417714i</t>
+  </si>
+  <si>
+    <t>0,0249220665305350i</t>
+  </si>
+  <si>
+    <t>0,0449493150766644i</t>
+  </si>
+  <si>
+    <t>0,00334135155942127i</t>
+  </si>
+  <si>
+    <t>0,0161405591591010i</t>
+  </si>
+  <si>
+    <t>0,0147168088765009i</t>
+  </si>
+  <si>
+    <t>0,0240614353751186i</t>
+  </si>
+  <si>
+    <t>0,0600578284271831i</t>
+  </si>
+  <si>
+    <t>0,0557137060162514i</t>
+  </si>
+  <si>
+    <t>0,0576761979708601i</t>
+  </si>
+  <si>
+    <t>0,0313627658604934i</t>
+  </si>
+  <si>
+    <t>0,0450616633017215i</t>
+  </si>
+  <si>
+    <t>0,0219000000000009i</t>
+  </si>
+  <si>
+    <t>0,00647537384417200i</t>
+  </si>
+  <si>
+    <t>0,0103582063281853i</t>
+  </si>
+  <si>
+    <t>0,0160651682077911i</t>
+  </si>
+  <si>
+    <t>0,0229735398846467i</t>
+  </si>
+  <si>
+    <t>0,0273590129753990i</t>
+  </si>
+  <si>
+    <t>0,00190530134637602i</t>
+  </si>
+  <si>
+    <t>0,00612086246397569i</t>
+  </si>
+  <si>
+    <t>0,0100594408408975i</t>
+  </si>
+  <si>
+    <t>0,0182481005295384i</t>
+  </si>
+  <si>
+    <t>0,0306994397072823i</t>
+  </si>
+  <si>
+    <t>0,00740246715153400i</t>
+  </si>
+  <si>
+    <t>0,0186549924506820i</t>
+  </si>
+  <si>
+    <t>0,00719652075305022i</t>
+  </si>
+  <si>
+    <t>0,00791430839937846i</t>
+  </si>
+  <si>
+    <t>0,0185158370548798i</t>
   </si>
 </sst>
 </file>
@@ -4156,10 +4450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q1026"/>
+  <dimension ref="A1:AB1026"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L57" workbookViewId="0">
-      <selection activeCell="AC65" sqref="AC65"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4172,9 +4466,16 @@
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
     <col min="11" max="11" width="17.1640625" customWidth="1"/>
     <col min="13" max="13" width="28.83203125" customWidth="1"/>
+    <col min="19" max="19" width="30.6640625" customWidth="1"/>
+    <col min="21" max="21" width="4" customWidth="1"/>
+    <col min="22" max="22" width="22" customWidth="1"/>
+    <col min="24" max="24" width="3.1640625" customWidth="1"/>
+    <col min="25" max="25" width="22.1640625" customWidth="1"/>
+    <col min="27" max="27" width="5.1640625" customWidth="1"/>
+    <col min="28" max="28" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -4205,8 +4506,20 @@
       <c r="Q1" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="S1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4255,8 +4568,35 @@
       <c r="Q2">
         <v>4.1921999999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T2">
+        <v>-4.5134999999999996</v>
+      </c>
+      <c r="U2" t="s">
+        <v>15</v>
+      </c>
+      <c r="V2" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2">
+        <v>7.4409999999999998</v>
+      </c>
+      <c r="X2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z2">
+        <v>-4.1921999999999997</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0</v>
       </c>
@@ -4306,8 +4646,35 @@
       <c r="Q3">
         <v>2.9806209331865099</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T3">
+        <v>-1.5376082997323099</v>
+      </c>
+      <c r="U3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V3" t="s">
+        <v>18</v>
+      </c>
+      <c r="W3">
+        <v>3.57721019566968</v>
+      </c>
+      <c r="X3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z3">
+        <v>-2.7179950986860502</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
@@ -4354,8 +4721,35 @@
       <c r="Q4">
         <v>65.384163267709297</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T4">
+        <v>-1.4474721294687301</v>
+      </c>
+      <c r="U4" t="s">
+        <v>17</v>
+      </c>
+      <c r="V4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W4">
+        <v>5.2050859951759199</v>
+      </c>
+      <c r="X4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z4">
+        <v>-29.900813739589701</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>1.6E-2</v>
       </c>
@@ -4387,8 +4781,35 @@
       <c r="Q5">
         <v>2.7963653543586799</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T5">
+        <v>-1.32410520712294</v>
+      </c>
+      <c r="U5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V5" t="s">
+        <v>20</v>
+      </c>
+      <c r="W5">
+        <v>0.89706846020109299</v>
+      </c>
+      <c r="X5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z5">
+        <v>-2.5749260146569002</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2.4E-2</v>
       </c>
@@ -4420,8 +4841,35 @@
       <c r="Q6">
         <v>0.73556810240083204</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T6">
+        <v>-1.27379667746776</v>
+      </c>
+      <c r="U6" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" t="s">
+        <v>21</v>
+      </c>
+      <c r="W6">
+        <v>5.78905737114468</v>
+      </c>
+      <c r="X6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z6">
+        <v>-0.67133982645586499</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>3.2000000000000001E-2</v>
       </c>
@@ -4453,8 +4901,35 @@
       <c r="Q7">
         <v>0.33517844129265301</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T7">
+        <v>-6.2856446869638098</v>
+      </c>
+      <c r="U7" t="s">
+        <v>17</v>
+      </c>
+      <c r="V7" t="s">
+        <v>22</v>
+      </c>
+      <c r="W7">
+        <v>1.9081374375228399</v>
+      </c>
+      <c r="X7" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z7">
+        <v>-0.33425062170057301</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0.04</v>
       </c>
@@ -4486,8 +4961,35 @@
       <c r="Q8">
         <v>0.13396872395327</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T8">
+        <v>2.28211175078073</v>
+      </c>
+      <c r="U8" t="s">
+        <v>15</v>
+      </c>
+      <c r="V8" t="s">
+        <v>23</v>
+      </c>
+      <c r="W8">
+        <v>10.3555223494981</v>
+      </c>
+      <c r="X8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z8">
+        <v>-0.126202924180885</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>4.8000000000000001E-2</v>
       </c>
@@ -4519,8 +5021,35 @@
       <c r="Q9">
         <v>0.19380254140433401</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T9">
+        <v>-2.1485033064700598</v>
+      </c>
+      <c r="U9" t="s">
+        <v>15</v>
+      </c>
+      <c r="V9" t="s">
+        <v>24</v>
+      </c>
+      <c r="W9">
+        <v>17.609173982636801</v>
+      </c>
+      <c r="X9" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z9">
+        <v>-0.19377373512562299</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>5.6000000000000001E-2</v>
       </c>
@@ -4552,8 +5081,35 @@
       <c r="Q10">
         <v>7.6317350898156305E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T10">
+        <v>-2.14289896449251</v>
+      </c>
+      <c r="U10" t="s">
+        <v>15</v>
+      </c>
+      <c r="V10" t="s">
+        <v>25</v>
+      </c>
+      <c r="W10">
+        <v>-13.7241428991584</v>
+      </c>
+      <c r="X10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z10">
+        <v>-7.4591020894903104E-2</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -4585,8 +5141,35 @@
       <c r="Q11">
         <v>6.9421835463110898E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T11">
+        <v>-2.0797373165935</v>
+      </c>
+      <c r="U11" t="s">
+        <v>15</v>
+      </c>
+      <c r="V11" t="s">
+        <v>26</v>
+      </c>
+      <c r="W11">
+        <v>-5.7214966386687403</v>
+      </c>
+      <c r="X11" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z11">
+        <v>-6.7843988499791105E-2</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>7.1999999999999995E-2</v>
       </c>
@@ -4618,8 +5201,35 @@
       <c r="Q12">
         <v>8.6246526878069496E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T12">
+        <v>-2.0462212645656699</v>
+      </c>
+      <c r="U12" t="s">
+        <v>15</v>
+      </c>
+      <c r="V12" t="s">
+        <v>27</v>
+      </c>
+      <c r="W12">
+        <v>-1.4243784915693001</v>
+      </c>
+      <c r="X12" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z12">
+        <v>-8.2822163254883396E-2</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>0.08</v>
       </c>
@@ -4651,8 +5261,35 @@
       <c r="Q13">
         <v>8.8466057156358802E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T13">
+        <v>-2.0086545058723799</v>
+      </c>
+      <c r="U13" t="s">
+        <v>15</v>
+      </c>
+      <c r="V13" t="s">
+        <v>28</v>
+      </c>
+      <c r="W13">
+        <v>-3.3902935690751201</v>
+      </c>
+      <c r="X13" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z13">
+        <v>-6.4956142999743893E-2</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>8.7999999999999995E-2</v>
       </c>
@@ -4684,8 +5321,35 @@
       <c r="Q14">
         <v>6.7316004139389804E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T14">
+        <v>-1.9717439134063699</v>
+      </c>
+      <c r="U14" t="s">
+        <v>15</v>
+      </c>
+      <c r="V14" t="s">
+        <v>29</v>
+      </c>
+      <c r="W14">
+        <v>-0.13090167484193499</v>
+      </c>
+      <c r="X14" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z14">
+        <v>-3.7781309866507497E-2</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>9.6000000000000002E-2</v>
       </c>
@@ -4717,8 +5381,35 @@
       <c r="Q15">
         <v>6.6653983966048602E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T15">
+        <v>-2.0002503868526298</v>
+      </c>
+      <c r="U15" t="s">
+        <v>15</v>
+      </c>
+      <c r="V15" t="s">
+        <v>30</v>
+      </c>
+      <c r="W15">
+        <v>-2.41266097234926</v>
+      </c>
+      <c r="X15" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z15">
+        <v>-3.3409725622525102E-2</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>0.104</v>
       </c>
@@ -4750,8 +5441,35 @@
       <c r="Q16">
         <v>3.21060499855267E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T16">
+        <v>-2.0405015495604899</v>
+      </c>
+      <c r="U16" t="s">
+        <v>15</v>
+      </c>
+      <c r="V16" t="s">
+        <v>31</v>
+      </c>
+      <c r="W16">
+        <v>1.30631709422368E-2</v>
+      </c>
+      <c r="X16" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z16">
+        <v>-6.86843237231099E-3</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>0.112</v>
       </c>
@@ -4783,8 +5501,35 @@
       <c r="Q17">
         <v>7.3500389081346706E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T17">
+        <v>-1.5992430385653</v>
+      </c>
+      <c r="U17" t="s">
+        <v>15</v>
+      </c>
+      <c r="V17" t="s">
+        <v>32</v>
+      </c>
+      <c r="W17">
+        <v>-1.6607120675804601</v>
+      </c>
+      <c r="X17" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z17">
+        <v>-5.80668037314922E-2</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>0.12</v>
       </c>
@@ -4816,8 +5561,35 @@
       <c r="Q18">
         <v>5.3033008588992098E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T18">
+        <v>-1.9146000000000001</v>
+      </c>
+      <c r="U18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V18" t="s">
+        <v>33</v>
+      </c>
+      <c r="W18">
+        <v>-0.162799999999999</v>
+      </c>
+      <c r="X18" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z18">
+        <v>-4.8300000000000697E-2</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>0.128</v>
       </c>
@@ -4849,8 +5621,35 @@
       <c r="Q19">
         <v>4.6569110686051497E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T19">
+        <v>-1.8577314201401001</v>
+      </c>
+      <c r="U19" t="s">
+        <v>15</v>
+      </c>
+      <c r="V19" t="s">
+        <v>34</v>
+      </c>
+      <c r="W19">
+        <v>-1.31740190873107</v>
+      </c>
+      <c r="X19" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z19">
+        <v>-4.61167171822532E-2</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>0.13600000000000001</v>
       </c>
@@ -4882,8 +5681,35 @@
       <c r="Q20">
         <v>2.44023809887032E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T20">
+        <v>-1.89865372653869</v>
+      </c>
+      <c r="U20" t="s">
+        <v>15</v>
+      </c>
+      <c r="V20" t="s">
+        <v>35</v>
+      </c>
+      <c r="W20">
+        <v>-0.47556099005439201</v>
+      </c>
+      <c r="X20" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z20">
+        <v>-2.2094880845584301E-2</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>0.14399999999999999</v>
       </c>
@@ -4915,8 +5741,35 @@
       <c r="Q21">
         <v>2.4009869728135E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T21">
+        <v>-1.8893076903608399</v>
+      </c>
+      <c r="U21" t="s">
+        <v>15</v>
+      </c>
+      <c r="V21" t="s">
+        <v>36</v>
+      </c>
+      <c r="W21">
+        <v>-0.60269412654857102</v>
+      </c>
+      <c r="X21" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z21">
+        <v>-1.7843324096630399E-2</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>0.152</v>
       </c>
@@ -4948,8 +5801,35 @@
       <c r="Q22">
         <v>4.9967300400527902E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T22">
+        <v>-1.9043408480368</v>
+      </c>
+      <c r="U22" t="s">
+        <v>15</v>
+      </c>
+      <c r="V22" t="s">
+        <v>37</v>
+      </c>
+      <c r="W22">
+        <v>-0.647749071492974</v>
+      </c>
+      <c r="X22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z22">
+        <v>-4.43728247296152E-2</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>0.16</v>
       </c>
@@ -4981,8 +5861,35 @@
       <c r="Q23">
         <v>2.89449898688805E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T23">
+        <v>-1.91712234782073</v>
+      </c>
+      <c r="U23" t="s">
+        <v>15</v>
+      </c>
+      <c r="V23" t="s">
+        <v>38</v>
+      </c>
+      <c r="W23">
+        <v>-0.31624959676957498</v>
+      </c>
+      <c r="X23" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z23">
+        <v>-9.4497009223330694E-3</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0.16800000000000001</v>
       </c>
@@ -5014,8 +5921,35 @@
       <c r="Q24">
         <v>3.5203098599034199E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T24">
+        <v>-1.92071720306827</v>
+      </c>
+      <c r="U24" t="s">
+        <v>15</v>
+      </c>
+      <c r="V24" t="s">
+        <v>39</v>
+      </c>
+      <c r="W24">
+        <v>-0.78078258533353395</v>
+      </c>
+      <c r="X24" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z24">
+        <v>-3.51515003627558E-2</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>0.17599999999999999</v>
       </c>
@@ -5047,8 +5981,35 @@
       <c r="Q25">
         <v>3.0726022265841299E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T25">
+        <v>-1.9040675764377999</v>
+      </c>
+      <c r="U25" t="s">
+        <v>15</v>
+      </c>
+      <c r="V25" t="s">
+        <v>40</v>
+      </c>
+      <c r="W25">
+        <v>-0.127468065305781</v>
+      </c>
+      <c r="X25" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z25">
+        <v>-3.0110189089045399E-2</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>0.184</v>
       </c>
@@ -5080,8 +6041,35 @@
       <c r="Q26">
         <v>3.2219589567340501E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T26">
+        <v>-1.9063010355074901</v>
+      </c>
+      <c r="U26" t="s">
+        <v>15</v>
+      </c>
+      <c r="V26" t="s">
+        <v>41</v>
+      </c>
+      <c r="W26">
+        <v>-0.67745710084162702</v>
+      </c>
+      <c r="X26" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z26">
+        <v>-3.0608979105098601E-2</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>0.192</v>
       </c>
@@ -5113,8 +6101,35 @@
       <c r="Q27">
         <v>4.23842430032456E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T27">
+        <v>-1.91686692121424</v>
+      </c>
+      <c r="U27" t="s">
+        <v>15</v>
+      </c>
+      <c r="V27" t="s">
+        <v>42</v>
+      </c>
+      <c r="W27">
+        <v>-0.189420718250771</v>
+      </c>
+      <c r="X27" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z27">
+        <v>-3.8254815148188098E-2</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>0.2</v>
       </c>
@@ -5146,8 +6161,35 @@
       <c r="Q28">
         <v>3.8119677511564497E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T28">
+        <v>-1.8703628526768901</v>
+      </c>
+      <c r="U28" t="s">
+        <v>15</v>
+      </c>
+      <c r="V28" t="s">
+        <v>43</v>
+      </c>
+      <c r="W28">
+        <v>-0.53776066855986704</v>
+      </c>
+      <c r="X28" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z28">
+        <v>-2.25976595081132E-2</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>0.20799999999999999</v>
       </c>
@@ -5179,8 +6221,35 @@
       <c r="Q29">
         <v>4.0058181481318601E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T29">
+        <v>-1.9063643750407</v>
+      </c>
+      <c r="U29" t="s">
+        <v>15</v>
+      </c>
+      <c r="V29" t="s">
+        <v>44</v>
+      </c>
+      <c r="W29">
+        <v>-0.28852444181263498</v>
+      </c>
+      <c r="X29" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z29">
+        <v>-3.9368278901429202E-2</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>0.216</v>
       </c>
@@ -5212,8 +6281,35 @@
       <c r="Q30">
         <v>2.801912218166E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T30">
+        <v>-1.89291856108906</v>
+      </c>
+      <c r="U30" t="s">
+        <v>15</v>
+      </c>
+      <c r="V30" t="s">
+        <v>45</v>
+      </c>
+      <c r="W30">
+        <v>-0.38080662480977101</v>
+      </c>
+      <c r="X30" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z30">
+        <v>-2.0906038948011799E-2</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>0.224</v>
       </c>
@@ -5245,8 +6341,35 @@
       <c r="Q31">
         <v>1.2660187043393001E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T31">
+        <v>-1.88783581882379</v>
+      </c>
+      <c r="U31" t="s">
+        <v>15</v>
+      </c>
+      <c r="V31" t="s">
+        <v>46</v>
+      </c>
+      <c r="W31">
+        <v>-0.41509351246315601</v>
+      </c>
+      <c r="X31" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z31">
+        <v>-1.04158737043329E-2</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>0.23200000000000001</v>
       </c>
@@ -5278,8 +6401,35 @@
       <c r="Q32">
         <v>1.8073641730904099E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T32">
+        <v>-1.90378302490199</v>
+      </c>
+      <c r="U32" t="s">
+        <v>15</v>
+      </c>
+      <c r="V32" t="s">
+        <v>47</v>
+      </c>
+      <c r="W32">
+        <v>-0.24238878009911899</v>
+      </c>
+      <c r="X32" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z32">
+        <v>-1.62486998857325E-2</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>0.24</v>
       </c>
@@ -5311,8 +6461,35 @@
       <c r="Q33">
         <v>3.69871688213501E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T33">
+        <v>-1.8921571019888901</v>
+      </c>
+      <c r="U33" t="s">
+        <v>15</v>
+      </c>
+      <c r="V33" t="s">
+        <v>48</v>
+      </c>
+      <c r="W33">
+        <v>-0.50637445847529206</v>
+      </c>
+      <c r="X33" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z33">
+        <v>-3.2018969933091099E-2</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>0.248</v>
       </c>
@@ -5344,8 +6521,35 @@
       <c r="Q34">
         <v>3.5200000000000599E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T34">
+        <v>-1.8973</v>
+      </c>
+      <c r="U34" t="s">
+        <v>15</v>
+      </c>
+      <c r="V34" t="s">
+        <v>16</v>
+      </c>
+      <c r="W34">
+        <v>-0.13619999999999999</v>
+      </c>
+      <c r="X34" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z34">
+        <v>-3.5200000000000599E-2</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>0.25600000000000001</v>
       </c>
@@ -5377,8 +6581,35 @@
       <c r="Q35">
         <v>3.69871688213501E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T35">
+        <v>-1.8921571019888901</v>
+      </c>
+      <c r="U35" t="s">
+        <v>17</v>
+      </c>
+      <c r="V35" t="s">
+        <v>48</v>
+      </c>
+      <c r="W35">
+        <v>-0.50637445847529206</v>
+      </c>
+      <c r="X35" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z35">
+        <v>-3.2018969933091099E-2</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>0.26400000000000001</v>
       </c>
@@ -5410,8 +6641,35 @@
       <c r="Q36">
         <v>1.8073641730904099E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T36">
+        <v>-1.90378302490199</v>
+      </c>
+      <c r="U36" t="s">
+        <v>17</v>
+      </c>
+      <c r="V36" t="s">
+        <v>47</v>
+      </c>
+      <c r="W36">
+        <v>-0.24238878009911899</v>
+      </c>
+      <c r="X36" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z36">
+        <v>-1.62486998857325E-2</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>0.27200000000000002</v>
       </c>
@@ -5443,8 +6701,35 @@
       <c r="Q37">
         <v>1.2660187043393001E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T37">
+        <v>-1.88783581882379</v>
+      </c>
+      <c r="U37" t="s">
+        <v>17</v>
+      </c>
+      <c r="V37" t="s">
+        <v>46</v>
+      </c>
+      <c r="W37">
+        <v>-0.41509351246315601</v>
+      </c>
+      <c r="X37" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z37">
+        <v>-1.04158737043329E-2</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>0.28000000000000003</v>
       </c>
@@ -5476,8 +6761,35 @@
       <c r="Q38">
         <v>2.801912218166E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T38">
+        <v>-1.89291856108906</v>
+      </c>
+      <c r="U38" t="s">
+        <v>17</v>
+      </c>
+      <c r="V38" t="s">
+        <v>45</v>
+      </c>
+      <c r="W38">
+        <v>-0.38080662480977101</v>
+      </c>
+      <c r="X38" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z38">
+        <v>-2.0906038948011799E-2</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>0.28799999999999998</v>
       </c>
@@ -5509,8 +6821,35 @@
       <c r="Q39">
         <v>4.0058181481318601E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T39">
+        <v>-1.9063643750407</v>
+      </c>
+      <c r="U39" t="s">
+        <v>17</v>
+      </c>
+      <c r="V39" t="s">
+        <v>44</v>
+      </c>
+      <c r="W39">
+        <v>-0.28852444181263498</v>
+      </c>
+      <c r="X39" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z39">
+        <v>-3.9368278901429202E-2</v>
+      </c>
+      <c r="AA39" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>0.29599999999999999</v>
       </c>
@@ -5542,8 +6881,35 @@
       <c r="Q40">
         <v>3.8119677511564497E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T40">
+        <v>-1.8703628526768901</v>
+      </c>
+      <c r="U40" t="s">
+        <v>17</v>
+      </c>
+      <c r="V40" t="s">
+        <v>43</v>
+      </c>
+      <c r="W40">
+        <v>-0.53776066855986704</v>
+      </c>
+      <c r="X40" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z40">
+        <v>-2.25976595081132E-2</v>
+      </c>
+      <c r="AA40" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB40" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>0.30399999999999999</v>
       </c>
@@ -5575,8 +6941,35 @@
       <c r="Q41">
         <v>4.23842430032456E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T41">
+        <v>-1.91686692121424</v>
+      </c>
+      <c r="U41" t="s">
+        <v>17</v>
+      </c>
+      <c r="V41" t="s">
+        <v>42</v>
+      </c>
+      <c r="W41">
+        <v>-0.189420718250771</v>
+      </c>
+      <c r="X41" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z41">
+        <v>-3.8254815148188098E-2</v>
+      </c>
+      <c r="AA41" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>0.312</v>
       </c>
@@ -5608,8 +7001,35 @@
       <c r="Q42">
         <v>3.2219589567340501E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T42">
+        <v>-1.9063010355074901</v>
+      </c>
+      <c r="U42" t="s">
+        <v>17</v>
+      </c>
+      <c r="V42" t="s">
+        <v>41</v>
+      </c>
+      <c r="W42">
+        <v>-0.67745710084162702</v>
+      </c>
+      <c r="X42" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z42">
+        <v>-3.0608979105098601E-2</v>
+      </c>
+      <c r="AA42" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>0.32</v>
       </c>
@@ -5641,8 +7061,35 @@
       <c r="Q43">
         <v>3.0726022265841299E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T43">
+        <v>-1.9040675764377999</v>
+      </c>
+      <c r="U43" t="s">
+        <v>17</v>
+      </c>
+      <c r="V43" t="s">
+        <v>40</v>
+      </c>
+      <c r="W43">
+        <v>-0.127468065305781</v>
+      </c>
+      <c r="X43" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z43">
+        <v>-3.0110189089045399E-2</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>0.32800000000000001</v>
       </c>
@@ -5674,8 +7121,35 @@
       <c r="Q44">
         <v>3.5203098599034199E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T44">
+        <v>-1.92071720306827</v>
+      </c>
+      <c r="U44" t="s">
+        <v>17</v>
+      </c>
+      <c r="V44" t="s">
+        <v>39</v>
+      </c>
+      <c r="W44">
+        <v>-0.78078258533353395</v>
+      </c>
+      <c r="X44" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z44">
+        <v>-3.51515003627558E-2</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>0.33600000000000002</v>
       </c>
@@ -5707,8 +7181,35 @@
       <c r="Q45">
         <v>2.89449898688805E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T45">
+        <v>-1.91712234782073</v>
+      </c>
+      <c r="U45" t="s">
+        <v>17</v>
+      </c>
+      <c r="V45" t="s">
+        <v>38</v>
+      </c>
+      <c r="W45">
+        <v>-0.31624959676957498</v>
+      </c>
+      <c r="X45" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z45">
+        <v>-9.4497009223330694E-3</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>0.34399999999999997</v>
       </c>
@@ -5740,8 +7241,35 @@
       <c r="Q46">
         <v>4.9967300400527902E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T46">
+        <v>-1.9043408480368</v>
+      </c>
+      <c r="U46" t="s">
+        <v>17</v>
+      </c>
+      <c r="V46" t="s">
+        <v>37</v>
+      </c>
+      <c r="W46">
+        <v>-0.647749071492974</v>
+      </c>
+      <c r="X46" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z46">
+        <v>-4.43728247296152E-2</v>
+      </c>
+      <c r="AA46" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>0.35199999999999998</v>
       </c>
@@ -5773,8 +7301,35 @@
       <c r="Q47">
         <v>2.4009869728135E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T47">
+        <v>-1.8893076903608399</v>
+      </c>
+      <c r="U47" t="s">
+        <v>17</v>
+      </c>
+      <c r="V47" t="s">
+        <v>36</v>
+      </c>
+      <c r="W47">
+        <v>-0.60269412654857102</v>
+      </c>
+      <c r="X47" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z47">
+        <v>-1.7843324096630399E-2</v>
+      </c>
+      <c r="AA47" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>0.36</v>
       </c>
@@ -5806,8 +7361,35 @@
       <c r="Q48">
         <v>2.44023809887032E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T48">
+        <v>-1.89865372653869</v>
+      </c>
+      <c r="U48" t="s">
+        <v>17</v>
+      </c>
+      <c r="V48" t="s">
+        <v>35</v>
+      </c>
+      <c r="W48">
+        <v>-0.47556099005439201</v>
+      </c>
+      <c r="X48" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z48">
+        <v>-2.2094880845584301E-2</v>
+      </c>
+      <c r="AA48" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>0.36799999999999999</v>
       </c>
@@ -5839,8 +7421,35 @@
       <c r="Q49">
         <v>4.6569110686051497E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T49">
+        <v>-1.8577314201401001</v>
+      </c>
+      <c r="U49" t="s">
+        <v>17</v>
+      </c>
+      <c r="V49" t="s">
+        <v>34</v>
+      </c>
+      <c r="W49">
+        <v>-1.31740190873107</v>
+      </c>
+      <c r="X49" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z49">
+        <v>-4.61167171822532E-2</v>
+      </c>
+      <c r="AA49" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>0.376</v>
       </c>
@@ -5872,8 +7481,35 @@
       <c r="Q50">
         <v>5.3033008588992098E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T50">
+        <v>-1.9146000000000001</v>
+      </c>
+      <c r="U50" t="s">
+        <v>17</v>
+      </c>
+      <c r="V50" t="s">
+        <v>33</v>
+      </c>
+      <c r="W50">
+        <v>-0.162799999999999</v>
+      </c>
+      <c r="X50" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z50">
+        <v>-4.8300000000000697E-2</v>
+      </c>
+      <c r="AA50" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>0.38400000000000001</v>
       </c>
@@ -5905,8 +7541,35 @@
       <c r="Q51">
         <v>7.3500389081346706E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T51">
+        <v>-1.5992430385653</v>
+      </c>
+      <c r="U51" t="s">
+        <v>17</v>
+      </c>
+      <c r="V51" t="s">
+        <v>32</v>
+      </c>
+      <c r="W51">
+        <v>-1.6607120675804601</v>
+      </c>
+      <c r="X51" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z51">
+        <v>-5.80668037314922E-2</v>
+      </c>
+      <c r="AA51" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>0.39200000000000002</v>
       </c>
@@ -5938,8 +7601,35 @@
       <c r="Q52">
         <v>3.21060499855267E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T52">
+        <v>-2.0405015495604899</v>
+      </c>
+      <c r="U52" t="s">
+        <v>17</v>
+      </c>
+      <c r="V52" t="s">
+        <v>31</v>
+      </c>
+      <c r="W52">
+        <v>1.30631709422368E-2</v>
+      </c>
+      <c r="X52" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z52">
+        <v>-6.86843237231099E-3</v>
+      </c>
+      <c r="AA52" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>0.4</v>
       </c>
@@ -5971,8 +7661,35 @@
       <c r="Q53">
         <v>6.6653983966048602E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T53">
+        <v>-2.0002503868526298</v>
+      </c>
+      <c r="U53" t="s">
+        <v>17</v>
+      </c>
+      <c r="V53" t="s">
+        <v>30</v>
+      </c>
+      <c r="W53">
+        <v>-2.41266097234926</v>
+      </c>
+      <c r="X53" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z53">
+        <v>-3.3409725622525102E-2</v>
+      </c>
+      <c r="AA53" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>0.40799999999999997</v>
       </c>
@@ -6004,8 +7721,35 @@
       <c r="Q54">
         <v>6.7316004139389804E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T54">
+        <v>-1.9717439134063699</v>
+      </c>
+      <c r="U54" t="s">
+        <v>17</v>
+      </c>
+      <c r="V54" t="s">
+        <v>29</v>
+      </c>
+      <c r="W54">
+        <v>-0.13090167484193499</v>
+      </c>
+      <c r="X54" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z54">
+        <v>-3.7781309866507497E-2</v>
+      </c>
+      <c r="AA54" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB54" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>0.41599999999999998</v>
       </c>
@@ -6037,8 +7781,35 @@
       <c r="Q55">
         <v>8.8466057156358802E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T55">
+        <v>-2.0086545058723799</v>
+      </c>
+      <c r="U55" t="s">
+        <v>17</v>
+      </c>
+      <c r="V55" t="s">
+        <v>28</v>
+      </c>
+      <c r="W55">
+        <v>-3.3902935690751201</v>
+      </c>
+      <c r="X55" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z55">
+        <v>-6.4956142999743893E-2</v>
+      </c>
+      <c r="AA55" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB55" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>0.42399999999999999</v>
       </c>
@@ -6070,8 +7841,35 @@
       <c r="Q56">
         <v>8.6246526878069496E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T56">
+        <v>-2.0462212645656699</v>
+      </c>
+      <c r="U56" t="s">
+        <v>17</v>
+      </c>
+      <c r="V56" t="s">
+        <v>27</v>
+      </c>
+      <c r="W56">
+        <v>-1.4243784915693001</v>
+      </c>
+      <c r="X56" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z56">
+        <v>-8.2822163254883396E-2</v>
+      </c>
+      <c r="AA56" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB56" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>0.432</v>
       </c>
@@ -6103,8 +7901,35 @@
       <c r="Q57">
         <v>6.9421835463110898E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T57">
+        <v>-2.0797373165935</v>
+      </c>
+      <c r="U57" t="s">
+        <v>17</v>
+      </c>
+      <c r="V57" t="s">
+        <v>26</v>
+      </c>
+      <c r="W57">
+        <v>-5.7214966386687403</v>
+      </c>
+      <c r="X57" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z57">
+        <v>-6.7843988499791105E-2</v>
+      </c>
+      <c r="AA57" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB57" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>0.44</v>
       </c>
@@ -6136,8 +7961,35 @@
       <c r="Q58">
         <v>7.6317350898156305E-2</v>
       </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T58">
+        <v>-2.14289896449251</v>
+      </c>
+      <c r="U58" t="s">
+        <v>17</v>
+      </c>
+      <c r="V58" t="s">
+        <v>25</v>
+      </c>
+      <c r="W58">
+        <v>-13.7241428991584</v>
+      </c>
+      <c r="X58" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z58">
+        <v>-7.4591020894903104E-2</v>
+      </c>
+      <c r="AA58" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>0.44800000000000001</v>
       </c>
@@ -6169,8 +8021,35 @@
       <c r="Q59">
         <v>0.19380254140433401</v>
       </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T59">
+        <v>-2.1485033064700598</v>
+      </c>
+      <c r="U59" t="s">
+        <v>17</v>
+      </c>
+      <c r="V59" t="s">
+        <v>24</v>
+      </c>
+      <c r="W59">
+        <v>17.609173982636801</v>
+      </c>
+      <c r="X59" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z59">
+        <v>-0.19377373512562299</v>
+      </c>
+      <c r="AA59" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB59" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>0.45600000000000002</v>
       </c>
@@ -6202,8 +8081,35 @@
       <c r="Q60">
         <v>0.13396872395327</v>
       </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T60">
+        <v>2.28211175078073</v>
+      </c>
+      <c r="U60" t="s">
+        <v>17</v>
+      </c>
+      <c r="V60" t="s">
+        <v>23</v>
+      </c>
+      <c r="W60">
+        <v>10.3555223494981</v>
+      </c>
+      <c r="X60" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z60">
+        <v>-0.126202924180885</v>
+      </c>
+      <c r="AA60" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB60" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>0.46400000000000002</v>
       </c>
@@ -6235,8 +8141,35 @@
       <c r="Q61">
         <v>0.33517844129265301</v>
       </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T61">
+        <v>-6.2856446869638098</v>
+      </c>
+      <c r="U61" t="s">
+        <v>15</v>
+      </c>
+      <c r="V61" t="s">
+        <v>22</v>
+      </c>
+      <c r="W61">
+        <v>1.9081374375228399</v>
+      </c>
+      <c r="X61" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z61">
+        <v>-0.33425062170057301</v>
+      </c>
+      <c r="AA61" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB61" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="62" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>0.47199999999999998</v>
       </c>
@@ -6268,8 +8201,35 @@
       <c r="Q62">
         <v>0.73556810240083204</v>
       </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T62">
+        <v>-1.27379667746776</v>
+      </c>
+      <c r="U62" t="s">
+        <v>15</v>
+      </c>
+      <c r="V62" t="s">
+        <v>21</v>
+      </c>
+      <c r="W62">
+        <v>5.78905737114468</v>
+      </c>
+      <c r="X62" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z62">
+        <v>-0.67133982645586499</v>
+      </c>
+      <c r="AA62" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB62" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="63" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>0.48</v>
       </c>
@@ -6301,8 +8261,35 @@
       <c r="Q63">
         <v>2.7963653543586799</v>
       </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T63">
+        <v>-1.32410520712294</v>
+      </c>
+      <c r="U63" t="s">
+        <v>15</v>
+      </c>
+      <c r="V63" t="s">
+        <v>20</v>
+      </c>
+      <c r="W63">
+        <v>0.89706846020109299</v>
+      </c>
+      <c r="X63" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z63">
+        <v>-2.5749260146569002</v>
+      </c>
+      <c r="AA63" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB63" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="64" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>0.48799999999999999</v>
       </c>
@@ -6334,8 +8321,35 @@
       <c r="Q64">
         <v>65.384163267709297</v>
       </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T64">
+        <v>-1.4474721294687301</v>
+      </c>
+      <c r="U64" t="s">
+        <v>15</v>
+      </c>
+      <c r="V64" t="s">
+        <v>19</v>
+      </c>
+      <c r="W64">
+        <v>5.2050859951759199</v>
+      </c>
+      <c r="X64" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z64">
+        <v>-29.900813739589701</v>
+      </c>
+      <c r="AA64" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB64" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>0.496</v>
       </c>
@@ -6367,8 +8381,35 @@
       <c r="Q65">
         <v>2.9806209331865099</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="T65">
+        <v>-1.5376082997323099</v>
+      </c>
+      <c r="U65" t="s">
+        <v>15</v>
+      </c>
+      <c r="V65" t="s">
+        <v>18</v>
+      </c>
+      <c r="W65">
+        <v>3.57721019566968</v>
+      </c>
+      <c r="X65" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z65">
+        <v>-2.7179950986860502</v>
+      </c>
+      <c r="AA65" t="s">
+        <v>15</v>
+      </c>
+      <c r="AB65" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>0.504</v>
       </c>
@@ -6376,7 +8417,7 @@
         <v>1.4719</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>0.51200000000000001</v>
       </c>
@@ -6384,7 +8425,7 @@
         <v>1.8328</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>0.52</v>
       </c>
@@ -6392,7 +8433,7 @@
         <v>1.6127</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>0.52800000000000002</v>
       </c>
@@ -6400,7 +8441,7 @@
         <v>0.89970000000000006</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>0.53600000000000003</v>
       </c>
@@ -6408,7 +8449,7 @@
         <v>-6.4299999999999996E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>0.54400000000000004</v>
       </c>
@@ -6416,7 +8457,7 @@
         <v>-1.0238</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>0.55200000000000005</v>
       </c>
@@ -6424,7 +8465,7 @@
         <v>-1.7193000000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>0.56000000000000005</v>
       </c>
@@ -6432,7 +8473,7 @@
         <v>-1.9305000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>0.56799999999999995</v>
       </c>
@@ -6440,7 +8481,7 @@
         <v>-1.5651999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>0.57599999999999996</v>
       </c>
@@ -6448,7 +8489,7 @@
         <v>-0.72889999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>0.58399999999999996</v>
       </c>
@@ -6456,7 +8497,7 @@
         <v>0.28789999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>0.59199999999999997</v>
       </c>
@@ -6464,7 +8505,7 @@
         <v>1.1901999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>0.6</v>
       </c>
@@ -6472,7 +8513,7 @@
         <v>1.7403999999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>0.60799999999999998</v>
       </c>
@@ -6480,7 +8521,7 @@
         <v>1.7667999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>0.61599999999999999</v>
       </c>

</xml_diff>